<commit_message>
feat: change jobName to id, excel revise
</commit_message>
<xml_diff>
--- a/public/template/staff/Template_Export_Staff_Payroll.xlsx
+++ b/public/template/staff/Template_Export_Staff_Payroll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\staff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2804419-EDAC-4709-B7C8-8EBDC42B3584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AEDE8F-092C-4A9D-A54C-12C840593721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
+    <workbookView xWindow="-22680" yWindow="1728" windowWidth="21600" windowHeight="11232" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Staff Payroll" sheetId="1" r:id="rId1"/>
@@ -25,36 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Payroll Date</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>Basic Income</t>
-  </si>
-  <si>
-    <t>Annual Increase Incentive</t>
-  </si>
-  <si>
-    <t>Absent</t>
-  </si>
-  <si>
-    <t>Late</t>
-  </si>
-  <si>
-    <t>Total Reduction</t>
-  </si>
-  <si>
-    <t>Net Income</t>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Tanggal Penggajian</t>
+  </si>
+  <si>
+    <t>Cabang</t>
+  </si>
+  <si>
+    <t>Penghasilan Pokok</t>
+  </si>
+  <si>
+    <t>Insentif Kenaikan Tahunan</t>
+  </si>
+  <si>
+    <t>Tidak Masuk Kerja</t>
+  </si>
+  <si>
+    <t>Keterlambatan</t>
+  </si>
+  <si>
+    <t>Total Pengurangan</t>
+  </si>
+  <si>
+    <t>Penerimaan Bersih</t>
+  </si>
+  <si>
+    <t>Total Penghasilan</t>
   </si>
 </sst>
 </file>
@@ -436,30 +439,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0BD312-7EF2-F445-B81C-635468D350A0}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="22.375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="21.125" customWidth="1"/>
     <col min="6" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="11.25" customWidth="1"/>
-    <col min="8" max="8" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="16.875" customWidth="1"/>
     <col min="9" max="9" width="22.375" customWidth="1"/>
     <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="11" width="15.25" customWidth="1"/>
+    <col min="11" max="11" width="20.625" customWidth="1"/>
     <col min="12" max="12" width="17.25" customWidth="1"/>
     <col min="13" max="13" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,9 +488,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: fix 2 issue
</commit_message>
<xml_diff>
--- a/public/template/staff/Template_Export_Staff_Payroll.xlsx
+++ b/public/template/staff/Template_Export_Staff_Payroll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\staff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AEDE8F-092C-4A9D-A54C-12C840593721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241252DD-8A10-4F11-A883-D8640BB9030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22680" yWindow="1728" windowWidth="21600" windowHeight="11232" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Staff Payroll" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Total Penghasilan</t>
+  </si>
+  <si>
+    <t>Kasbon</t>
   </si>
 </sst>
 </file>
@@ -439,30 +442,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0BD312-7EF2-F445-B81C-635468D350A0}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="22.375" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="22.3984375" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="21.125" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="17.75" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
-    <col min="9" max="9" width="22.375" customWidth="1"/>
+    <col min="5" max="5" width="21.09765625" customWidth="1"/>
+    <col min="6" max="6" width="24.8984375" customWidth="1"/>
+    <col min="7" max="7" width="17.69921875" customWidth="1"/>
+    <col min="8" max="8" width="16.8984375" customWidth="1"/>
+    <col min="9" max="9" width="22.3984375" customWidth="1"/>
     <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="11" width="20.625" customWidth="1"/>
-    <col min="12" max="12" width="17.25" customWidth="1"/>
-    <col min="13" max="13" width="17.75" customWidth="1"/>
+    <col min="11" max="11" width="20.59765625" customWidth="1"/>
+    <col min="12" max="12" width="17.19921875" customWidth="1"/>
+    <col min="13" max="13" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,12 +491,15 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>